<commit_message>
Add project settings dialog for low stock and expiry thresholds
</commit_message>
<xml_diff>
--- a/projects/pepsi_Transactions.xlsx
+++ b/projects/pepsi_Transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K127"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6520,6 +6520,43 @@
       </c>
       <c r="K127" t="inlineStr"/>
     </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>1765302810</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>pepsi</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2025-12-09 19:53:30</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>تست</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>اول</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>دخول</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>9</v>
+      </c>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>